<commit_message>
Assignment: Use cases and scenario
</commit_message>
<xml_diff>
--- a/Daniel/Use Case specification.xlsx
+++ b/Daniel/Use Case specification.xlsx
@@ -5,21 +5,22 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DanielFelipe\Documents\Daniel\Dropbox\PoliMi\Semestre 1\Software engineering 2\Project\SE2-PoliMi-MyTaxi\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DanielFelipe\Documents\Daniel\Dropbox\PoliMi\Semestre 1\Software engineering 2\Project\SE2-PoliMi-MyTaxi\Daniel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4395" yWindow="645" windowWidth="16590" windowHeight="8415"/>
+    <workbookView xWindow="4395" yWindow="645" windowWidth="16590" windowHeight="8415" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="UC-01" sheetId="1" r:id="rId1"/>
+    <sheet name="UC-02" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
   <si>
     <t>No.</t>
   </si>
@@ -54,9 +55,6 @@
     <t>Exit condition</t>
   </si>
   <si>
-    <t>Actor</t>
-  </si>
-  <si>
     <t>System</t>
   </si>
   <si>
@@ -67,6 +65,269 @@
   </si>
   <si>
     <t>Related scenarios</t>
+  </si>
+  <si>
+    <t>Request taxi service</t>
+  </si>
+  <si>
+    <t>The passenger is waiting for the taxi driver, who will arrive at the specified origin within the informed estimated arrival time.</t>
+  </si>
+  <si>
+    <t>Passenger</t>
+  </si>
+  <si>
+    <t>Taxi driver</t>
+  </si>
+  <si>
+    <t>Passenger, Taxi driver</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The passenger is in the MyTaxiService's web site or has launched the MyTaxiService mobile application.
+The taxi driver has informed the system that he is available.
+The passenger selects the option </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Request for taxi service</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Asks the passenger to provide the </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>request for service</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>information</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Identifies the zone that corresponds to the specified origin position.</t>
+  </si>
+  <si>
+    <t>Checks if the received information is correct and complete.</t>
+  </si>
+  <si>
+    <t>Informs the system that he accepts the request.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Sends the </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>accepted request information</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to the passenger.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Replies the system with the the </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>request for service information</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Sends the </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>incoming request information</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to the first available taxi driver in the zone's queue.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Receives the </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>accepted request information.</t>
+    </r>
+  </si>
+  <si>
+    <t>3.1. The received information is not correct or complete:
+- The system informs the passenger that the sent information is wrong or incomplete.
+- Return to step 1.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Builds the </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>incoming request information.</t>
+    </r>
+  </si>
+  <si>
+    <t>6.1. The zone's queue is empty or every taxi driver cancels the request:
+- The system informs the passenger(s) that it is impossible to find a taxi driver.
+- The Use Case ends.</t>
+  </si>
+  <si>
+    <t>7.1. The taxi driver does not accept the request:
+- The system sends the taxi driver to the end of the zone's queue.
+- Return to step 6.</t>
+  </si>
+  <si>
+    <t>UC-02</t>
+  </si>
+  <si>
+    <t>Authenticate</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The taxi driver is already registered in MyTaxiService.
+The taxi driver has not logged in MyTaxiService yet.
+The taxi driver has launched the MyTaxiService mobile application.
+The taxi driver selects the option </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Log in</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>The taxi driver is logged in the MyTaxiService mobile application.</t>
+  </si>
+  <si>
+    <t>Asks the taxi driver his username and password.</t>
+  </si>
+  <si>
+    <t>Replies the system with his username and password.</t>
+  </si>
+  <si>
+    <t>Checks that received information is complete and correct.</t>
+  </si>
+  <si>
+    <t>Logs the taxi driver in the MyTaxiService mobile appplication.</t>
+  </si>
+  <si>
+    <t>3.1. The received information is not correct or complete:
+- The system informs the taxi driver that the sent information is wrong or incomplete.
+- Return to step 1.</t>
   </si>
 </sst>
 </file>
@@ -116,13 +377,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -197,6 +451,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -224,7 +485,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -452,11 +713,168 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color theme="3"/>
+      </left>
+      <right style="thin">
+        <color theme="3"/>
+      </right>
+      <top style="thin">
+        <color theme="3"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="3"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="3"/>
+      </top>
+      <bottom style="thin">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="3"/>
+      </right>
+      <top style="thin">
+        <color theme="3"/>
+      </top>
+      <bottom style="thin">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="3"/>
+      </right>
+      <top style="thin">
+        <color theme="3"/>
+      </top>
+      <bottom style="thin">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="3"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="3"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="3"/>
+      </right>
+      <top style="thin">
+        <color theme="3"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="3"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="3"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="3"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color theme="3"/>
+      </top>
+      <bottom style="thin">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="3"/>
+      </top>
+      <bottom style="thin">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="3"/>
+      </right>
+      <top style="medium">
+        <color theme="3"/>
+      </top>
+      <bottom style="thin">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="3"/>
+      </top>
+      <bottom style="thin">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="3"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="3"/>
+      </top>
+      <bottom style="thin">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -480,108 +898,177 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -893,25 +1380,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:I30"/>
+  <dimension ref="B1:I38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10:F10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2" style="3" customWidth="1"/>
     <col min="2" max="2" width="21.5703125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="18" style="3" customWidth="1"/>
-    <col min="4" max="4" width="24" style="3" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="27.85546875" style="3" customWidth="1"/>
-    <col min="7" max="9" width="10.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="20" style="3" customWidth="1"/>
+    <col min="5" max="5" width="10" style="3" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="23.5703125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" style="3" customWidth="1"/>
     <col min="10" max="16384" width="17.28515625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:9" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="19" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="1"/>
@@ -930,14 +1421,16 @@
       <c r="B4" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="45" t="s">
+      <c r="C4" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="40"/>
+      <c r="D4" s="21"/>
       <c r="E4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="12"/>
+      <c r="F4" s="43">
+        <v>42303</v>
+      </c>
       <c r="H4" s="5"/>
       <c r="I4" s="4"/>
     </row>
@@ -951,72 +1444,80 @@
       <c r="I5" s="4"/>
     </row>
     <row r="6" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="14" t="str">
+      <c r="C6" s="13" t="str">
         <f>B2</f>
         <v>UC-01</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="32"/>
-      <c r="F6" s="33"/>
-      <c r="H6" s="19"/>
+      <c r="E6" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="31"/>
+      <c r="H6" s="18"/>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="2:9" s="18" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="B7" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="44"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="41"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
+    <row r="7" spans="2:9" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="B7" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="27"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="29"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
     </row>
     <row r="8" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="44"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="41"/>
-      <c r="H8" s="19"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="29"/>
+      <c r="H8" s="18"/>
       <c r="I8" s="4"/>
     </row>
     <row r="9" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="43"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="41"/>
-      <c r="H9" s="19"/>
-    </row>
-    <row r="10" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="42" t="s">
+      <c r="C9" s="36"/>
+      <c r="D9" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="21"/>
+      <c r="F9" s="29"/>
+      <c r="H9" s="18"/>
+    </row>
+    <row r="10" spans="2:9" s="45" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="43"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="41"/>
-      <c r="H10" s="19"/>
-    </row>
-    <row r="11" spans="2:9" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="21" t="s">
+      <c r="C10" s="44"/>
+      <c r="D10" s="47" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="48"/>
+      <c r="F10" s="49"/>
+      <c r="H10" s="46"/>
+    </row>
+    <row r="11" spans="2:9" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="22"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="25"/>
-      <c r="H11" s="19"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="50" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="51"/>
+      <c r="F11" s="52"/>
+      <c r="H11" s="18"/>
     </row>
     <row r="12" spans="2:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="8"/>
@@ -1024,156 +1525,309 @@
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
-      <c r="H12" s="19"/>
+      <c r="H12" s="18"/>
     </row>
     <row r="13" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="58" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="59"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="59"/>
+      <c r="F13" s="59"/>
+      <c r="G13" s="59"/>
+      <c r="H13" s="60"/>
+      <c r="I13" s="17"/>
+    </row>
+    <row r="14" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="54" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="55"/>
+      <c r="E14" s="54" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="55"/>
+      <c r="G14" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" s="34"/>
+    </row>
+    <row r="15" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="41"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="57"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="57"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="34"/>
+    </row>
+    <row r="16" spans="2:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="15">
+        <v>1</v>
+      </c>
+      <c r="C16" s="20"/>
+      <c r="D16" s="66"/>
+      <c r="E16" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" s="66"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="67"/>
+    </row>
+    <row r="17" spans="2:8" s="17" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="53">
+        <v>2</v>
+      </c>
+      <c r="C17" s="68" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="69"/>
+      <c r="E17" s="68"/>
+      <c r="F17" s="69"/>
+      <c r="G17" s="68"/>
+      <c r="H17" s="70"/>
+    </row>
+    <row r="18" spans="2:8" s="17" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="15">
+        <v>3</v>
+      </c>
+      <c r="C18" s="68"/>
+      <c r="D18" s="69"/>
+      <c r="E18" s="68" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" s="69"/>
+      <c r="G18" s="68"/>
+      <c r="H18" s="70"/>
+    </row>
+    <row r="19" spans="2:8" s="17" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="53">
+        <v>4</v>
+      </c>
+      <c r="C19" s="68"/>
+      <c r="D19" s="69"/>
+      <c r="E19" s="68" t="s">
+        <v>22</v>
+      </c>
+      <c r="F19" s="69"/>
+      <c r="G19" s="68"/>
+      <c r="H19" s="70"/>
+    </row>
+    <row r="20" spans="2:8" s="17" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="53">
+        <v>5</v>
+      </c>
+      <c r="C20" s="68"/>
+      <c r="D20" s="69"/>
+      <c r="E20" s="68" t="s">
+        <v>30</v>
+      </c>
+      <c r="F20" s="69"/>
+      <c r="G20" s="68"/>
+      <c r="H20" s="70"/>
+    </row>
+    <row r="21" spans="2:8" s="17" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="15">
+        <v>6</v>
+      </c>
+      <c r="C21" s="68"/>
+      <c r="D21" s="69"/>
+      <c r="E21" s="68" t="s">
+        <v>27</v>
+      </c>
+      <c r="F21" s="69"/>
+      <c r="G21" s="68"/>
+      <c r="H21" s="70"/>
+    </row>
+    <row r="22" spans="2:8" s="17" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="53">
+        <v>7</v>
+      </c>
+      <c r="C22" s="68"/>
+      <c r="D22" s="69"/>
+      <c r="E22" s="68"/>
+      <c r="F22" s="69"/>
+      <c r="G22" s="68" t="s">
+        <v>24</v>
+      </c>
+      <c r="H22" s="70"/>
+    </row>
+    <row r="23" spans="2:8" s="17" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="15">
+        <v>8</v>
+      </c>
+      <c r="C23" s="68"/>
+      <c r="D23" s="69"/>
+      <c r="E23" s="68" t="s">
+        <v>25</v>
+      </c>
+      <c r="F23" s="69"/>
+      <c r="G23" s="68"/>
+      <c r="H23" s="70"/>
+    </row>
+    <row r="24" spans="2:8" s="17" customFormat="1" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="16">
+        <v>9</v>
+      </c>
+      <c r="C24" s="63" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" s="65"/>
+      <c r="E24" s="63"/>
+      <c r="F24" s="65"/>
+      <c r="G24" s="63"/>
+      <c r="H24" s="64"/>
+    </row>
+    <row r="25" spans="2:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="8"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+    </row>
+    <row r="26" spans="2:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="28"/>
-      <c r="H13" s="19"/>
-    </row>
-    <row r="14" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="C14" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="38"/>
-      <c r="E14" s="36" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" s="37"/>
-    </row>
-    <row r="15" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="30"/>
-      <c r="C15" s="38"/>
-      <c r="D15" s="38"/>
-      <c r="E15" s="38"/>
-      <c r="F15" s="37"/>
-    </row>
-    <row r="16" spans="2:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="16">
-        <v>1</v>
-      </c>
-      <c r="C16" s="34"/>
-      <c r="D16" s="46"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="35"/>
-    </row>
-    <row r="17" spans="2:6" s="18" customFormat="1" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="17">
-        <v>2</v>
-      </c>
-      <c r="C17" s="50"/>
-      <c r="D17" s="50"/>
-      <c r="E17" s="50"/>
-      <c r="F17" s="51"/>
-    </row>
-    <row r="18" spans="2:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="8"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-    </row>
-    <row r="19" spans="2:6" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="27"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-    </row>
-    <row r="20" spans="2:6" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="47"/>
-      <c r="C20" s="48"/>
-      <c r="D20" s="49"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-    </row>
-    <row r="21" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-    </row>
-    <row r="22" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-    </row>
-    <row r="23" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-    </row>
-    <row r="24" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-    </row>
-    <row r="25" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-    </row>
-    <row r="26" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-    </row>
-    <row r="27" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="10"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
+      <c r="C26" s="38"/>
+      <c r="D26" s="39"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+    </row>
+    <row r="27" spans="2:8" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="72" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" s="73"/>
+      <c r="D27" s="74"/>
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
     </row>
-    <row r="28" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
+    <row r="28" spans="2:8" s="17" customFormat="1" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="72" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" s="73"/>
+      <c r="D28" s="74"/>
       <c r="E28" s="9"/>
       <c r="F28" s="9"/>
     </row>
-    <row r="29" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
+    <row r="29" spans="2:8" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="72" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="73"/>
+      <c r="D29" s="74"/>
       <c r="E29" s="9"/>
       <c r="F29" s="9"/>
     </row>
-    <row r="30" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
+    <row r="30" spans="2:8" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="71"/>
+      <c r="C30" s="51"/>
+      <c r="D30" s="52"/>
       <c r="E30" s="9"/>
       <c r="F30" s="9"/>
     </row>
+    <row r="31" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+    </row>
+    <row r="32" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+    </row>
+    <row r="33" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+    </row>
+    <row r="34" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+    </row>
+    <row r="35" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+    </row>
+    <row r="36" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+    </row>
+    <row r="37" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+    </row>
+    <row r="38" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B38" s="10"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+    </row>
   </sheetData>
-  <mergeCells count="22">
+  <mergeCells count="49">
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B13:H13"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="G14:H15"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:F21"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C16:D16"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:F17"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="D7:F7"/>
     <mergeCell ref="E6:F6"/>
@@ -1185,12 +1839,316 @@
     <mergeCell ref="C14:D15"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B8:C8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:G34"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="2" style="17" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" style="17" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" style="17" customWidth="1"/>
+    <col min="4" max="4" width="20" style="17" customWidth="1"/>
+    <col min="5" max="5" width="10" style="17" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" style="17" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" style="17" customWidth="1"/>
+    <col min="8" max="16384" width="17.28515625" style="17"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:7" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:7" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B2" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+    </row>
+    <row r="4" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="21"/>
+      <c r="E4" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="43">
+        <v>42303</v>
+      </c>
+      <c r="G4" s="18"/>
+    </row>
+    <row r="5" spans="2:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="6"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="18"/>
+    </row>
+    <row r="6" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="13" t="str">
+        <f>B2</f>
+        <v>UC-02</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="31"/>
+      <c r="G6" s="18"/>
+    </row>
+    <row r="7" spans="2:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="B7" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="27"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="18"/>
+    </row>
+    <row r="8" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="27"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="18"/>
+    </row>
+    <row r="9" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="36"/>
+      <c r="D9" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="21"/>
+      <c r="F9" s="29"/>
+    </row>
+    <row r="10" spans="2:7" s="45" customFormat="1" ht="76.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="44"/>
+      <c r="D10" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="48"/>
+      <c r="F10" s="49"/>
+    </row>
+    <row r="11" spans="2:7" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="61" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="62"/>
+      <c r="D11" s="50" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="51"/>
+      <c r="F11" s="52"/>
+    </row>
+    <row r="12" spans="2:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="8"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+    </row>
+    <row r="13" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="39"/>
+    </row>
+    <row r="14" spans="2:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="35"/>
+      <c r="E14" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="34"/>
+    </row>
+    <row r="15" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="41"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="34"/>
+    </row>
+    <row r="16" spans="2:7" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="15">
+        <v>1</v>
+      </c>
+      <c r="C16" s="22"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="F16" s="32"/>
+    </row>
+    <row r="17" spans="2:6" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="53">
+        <v>2</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="23"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="32"/>
+    </row>
+    <row r="18" spans="2:6" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="53">
+        <v>3</v>
+      </c>
+      <c r="C18" s="22"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="F18" s="32"/>
+    </row>
+    <row r="19" spans="2:6" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="16">
+        <v>4</v>
+      </c>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="F19" s="25"/>
+    </row>
+    <row r="20" spans="2:6" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="8"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+    </row>
+    <row r="21" spans="2:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="38"/>
+      <c r="D21" s="39"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+    </row>
+    <row r="22" spans="2:6" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="71" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="51"/>
+      <c r="D22" s="52"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+    </row>
+    <row r="23" spans="2:6" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+    </row>
+    <row r="24" spans="2:6" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+    </row>
+    <row r="25" spans="2:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+    </row>
+    <row r="26" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+    </row>
+    <row r="27" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+    </row>
+    <row r="28" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <mergeCells count="26">
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:D15"/>
+    <mergeCell ref="E14:F15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
     <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:F10"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="D11:F11"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Assignment of requirements. UC specification correction
</commit_message>
<xml_diff>
--- a/Daniel/Use Case specification.xlsx
+++ b/Daniel/Use Case specification.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4395" yWindow="645" windowWidth="16590" windowHeight="8415" activeTab="1"/>
+    <workbookView xWindow="4395" yWindow="645" windowWidth="16590" windowHeight="8415"/>
   </bookViews>
   <sheets>
     <sheet name="UC-01" sheetId="1" r:id="rId1"/>
@@ -921,24 +921,101 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -951,124 +1028,47 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1382,9 +1382,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I38"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10:F10"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1421,14 +1419,14 @@
       <c r="B4" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="21"/>
+      <c r="D4" s="54"/>
       <c r="E4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="43">
+      <c r="F4" s="20">
         <v>42303</v>
       </c>
       <c r="H4" s="5"/>
@@ -1454,69 +1452,69 @@
       <c r="D6" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="30" t="s">
+      <c r="E6" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="31"/>
+      <c r="F6" s="60"/>
       <c r="H6" s="18"/>
       <c r="I6" s="4"/>
     </row>
     <row r="7" spans="2:9" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="27"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="29"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="58"/>
       <c r="H7" s="18"/>
       <c r="I7" s="18"/>
     </row>
     <row r="8" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="27"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="29"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="58"/>
       <c r="H8" s="18"/>
       <c r="I8" s="4"/>
     </row>
     <row r="9" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="36"/>
-      <c r="D9" s="28" t="s">
+      <c r="C9" s="45"/>
+      <c r="D9" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="21"/>
-      <c r="F9" s="29"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="58"/>
       <c r="H9" s="18"/>
     </row>
-    <row r="10" spans="2:9" s="45" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="26" t="s">
+    <row r="10" spans="2:9" s="21" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="44"/>
-      <c r="D10" s="47" t="s">
+      <c r="C10" s="68"/>
+      <c r="D10" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="48"/>
-      <c r="F10" s="49"/>
-      <c r="H10" s="46"/>
+      <c r="E10" s="66"/>
+      <c r="F10" s="67"/>
+      <c r="H10" s="22"/>
     </row>
     <row r="11" spans="2:9" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="61" t="s">
+      <c r="B11" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="62"/>
-      <c r="D11" s="50" t="s">
+      <c r="C11" s="47"/>
+      <c r="D11" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="51"/>
-      <c r="F11" s="52"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="29"/>
       <c r="H11" s="18"/>
     </row>
     <row r="12" spans="2:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1528,159 +1526,159 @@
       <c r="H12" s="18"/>
     </row>
     <row r="13" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="58" t="s">
+      <c r="B13" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="59"/>
-      <c r="D13" s="59"/>
-      <c r="E13" s="59"/>
-      <c r="F13" s="59"/>
-      <c r="G13" s="59"/>
-      <c r="H13" s="60"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="32"/>
       <c r="I13" s="17"/>
     </row>
     <row r="14" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="40" t="s">
+      <c r="B14" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="54" t="s">
+      <c r="C14" s="61" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="55"/>
-      <c r="E14" s="54" t="s">
+      <c r="D14" s="62"/>
+      <c r="E14" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="55"/>
-      <c r="G14" s="33" t="s">
+      <c r="F14" s="62"/>
+      <c r="G14" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="H14" s="34"/>
+      <c r="H14" s="39"/>
     </row>
     <row r="15" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="41"/>
-      <c r="C15" s="56"/>
-      <c r="D15" s="57"/>
-      <c r="E15" s="56"/>
-      <c r="F15" s="57"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="34"/>
+      <c r="B15" s="53"/>
+      <c r="C15" s="63"/>
+      <c r="D15" s="64"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="64"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="39"/>
     </row>
     <row r="16" spans="2:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="15">
         <v>1</v>
       </c>
-      <c r="C16" s="20"/>
-      <c r="D16" s="66"/>
-      <c r="E16" s="20" t="s">
+      <c r="C16" s="41"/>
+      <c r="D16" s="55"/>
+      <c r="E16" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="F16" s="66"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="67"/>
+      <c r="F16" s="55"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="42"/>
     </row>
     <row r="17" spans="2:8" s="17" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="53">
+      <c r="B17" s="23">
         <v>2</v>
       </c>
-      <c r="C17" s="68" t="s">
+      <c r="C17" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="69"/>
-      <c r="E17" s="68"/>
-      <c r="F17" s="69"/>
-      <c r="G17" s="68"/>
-      <c r="H17" s="70"/>
+      <c r="D17" s="35"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="35"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="34"/>
     </row>
     <row r="18" spans="2:8" s="17" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="15">
         <v>3</v>
       </c>
-      <c r="C18" s="68"/>
-      <c r="D18" s="69"/>
-      <c r="E18" s="68" t="s">
+      <c r="C18" s="33"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="F18" s="69"/>
-      <c r="G18" s="68"/>
-      <c r="H18" s="70"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="34"/>
     </row>
     <row r="19" spans="2:8" s="17" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="53">
+      <c r="B19" s="23">
         <v>4</v>
       </c>
-      <c r="C19" s="68"/>
-      <c r="D19" s="69"/>
-      <c r="E19" s="68" t="s">
+      <c r="C19" s="33"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="F19" s="69"/>
-      <c r="G19" s="68"/>
-      <c r="H19" s="70"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="34"/>
     </row>
     <row r="20" spans="2:8" s="17" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="53">
+      <c r="B20" s="23">
         <v>5</v>
       </c>
-      <c r="C20" s="68"/>
-      <c r="D20" s="69"/>
-      <c r="E20" s="68" t="s">
+      <c r="C20" s="33"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="F20" s="69"/>
-      <c r="G20" s="68"/>
-      <c r="H20" s="70"/>
+      <c r="F20" s="35"/>
+      <c r="G20" s="33"/>
+      <c r="H20" s="34"/>
     </row>
     <row r="21" spans="2:8" s="17" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="15">
         <v>6</v>
       </c>
-      <c r="C21" s="68"/>
-      <c r="D21" s="69"/>
-      <c r="E21" s="68" t="s">
+      <c r="C21" s="33"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="F21" s="69"/>
-      <c r="G21" s="68"/>
-      <c r="H21" s="70"/>
+      <c r="F21" s="35"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="34"/>
     </row>
     <row r="22" spans="2:8" s="17" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="53">
+      <c r="B22" s="23">
         <v>7</v>
       </c>
-      <c r="C22" s="68"/>
-      <c r="D22" s="69"/>
-      <c r="E22" s="68"/>
-      <c r="F22" s="69"/>
-      <c r="G22" s="68" t="s">
+      <c r="C22" s="33"/>
+      <c r="D22" s="35"/>
+      <c r="E22" s="33"/>
+      <c r="F22" s="35"/>
+      <c r="G22" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="H22" s="70"/>
+      <c r="H22" s="34"/>
     </row>
     <row r="23" spans="2:8" s="17" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="15">
         <v>8</v>
       </c>
-      <c r="C23" s="68"/>
-      <c r="D23" s="69"/>
-      <c r="E23" s="68" t="s">
+      <c r="C23" s="33"/>
+      <c r="D23" s="35"/>
+      <c r="E23" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="F23" s="69"/>
-      <c r="G23" s="68"/>
-      <c r="H23" s="70"/>
+      <c r="F23" s="35"/>
+      <c r="G23" s="33"/>
+      <c r="H23" s="34"/>
     </row>
     <row r="24" spans="2:8" s="17" customFormat="1" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B24" s="16">
         <v>9</v>
       </c>
-      <c r="C24" s="63" t="s">
+      <c r="C24" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="D24" s="65"/>
-      <c r="E24" s="63"/>
-      <c r="F24" s="65"/>
-      <c r="G24" s="63"/>
-      <c r="H24" s="64"/>
+      <c r="D24" s="37"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="37"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="43"/>
     </row>
     <row r="25" spans="2:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="8"/>
@@ -1690,45 +1688,45 @@
       <c r="F25" s="4"/>
     </row>
     <row r="26" spans="2:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="37" t="s">
+      <c r="B26" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="C26" s="38"/>
-      <c r="D26" s="39"/>
+      <c r="C26" s="50"/>
+      <c r="D26" s="51"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
     </row>
     <row r="27" spans="2:8" ht="63" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="72" t="s">
+      <c r="B27" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="73"/>
-      <c r="D27" s="74"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="26"/>
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
     </row>
     <row r="28" spans="2:8" s="17" customFormat="1" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="72" t="s">
+      <c r="B28" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="73"/>
-      <c r="D28" s="74"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="26"/>
       <c r="E28" s="9"/>
       <c r="F28" s="9"/>
     </row>
     <row r="29" spans="2:8" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="72" t="s">
+      <c r="B29" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="C29" s="73"/>
-      <c r="D29" s="74"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="26"/>
       <c r="E29" s="9"/>
       <c r="F29" s="9"/>
     </row>
     <row r="30" spans="2:8" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="71"/>
-      <c r="C30" s="51"/>
-      <c r="D30" s="52"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="28"/>
+      <c r="D30" s="29"/>
       <c r="E30" s="9"/>
       <c r="F30" s="9"/>
     </row>
@@ -1790,6 +1788,39 @@
     </row>
   </sheetData>
   <mergeCells count="49">
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E14:F15"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="C14:D15"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G24:H24"/>
     <mergeCell ref="B28:D28"/>
     <mergeCell ref="B29:D29"/>
     <mergeCell ref="B30:D30"/>
@@ -1806,39 +1837,6 @@
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="G17:H17"/>
     <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E14:F15"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="C14:D15"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B8:C8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1849,7 +1847,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1884,14 +1882,14 @@
       <c r="B4" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="21"/>
+      <c r="D4" s="54"/>
       <c r="E4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="43">
+      <c r="F4" s="20">
         <v>42303</v>
       </c>
       <c r="G4" s="18"/>
@@ -1915,64 +1913,64 @@
       <c r="D6" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="30" t="s">
+      <c r="E6" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="31"/>
+      <c r="F6" s="60"/>
       <c r="G6" s="18"/>
     </row>
     <row r="7" spans="2:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="27"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="29"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="58"/>
       <c r="G7" s="18"/>
     </row>
     <row r="8" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="27"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="29"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="58"/>
       <c r="G8" s="18"/>
     </row>
     <row r="9" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="36"/>
-      <c r="D9" s="28" t="s">
+      <c r="C9" s="45"/>
+      <c r="D9" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="21"/>
-      <c r="F9" s="29"/>
-    </row>
-    <row r="10" spans="2:7" s="45" customFormat="1" ht="76.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="26" t="s">
+      <c r="E9" s="54"/>
+      <c r="F9" s="58"/>
+    </row>
+    <row r="10" spans="2:7" s="21" customFormat="1" ht="76.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="44"/>
-      <c r="D10" s="47" t="s">
+      <c r="C10" s="68"/>
+      <c r="D10" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="48"/>
-      <c r="F10" s="49"/>
+      <c r="E10" s="66"/>
+      <c r="F10" s="67"/>
     </row>
     <row r="11" spans="2:7" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="61" t="s">
+      <c r="B11" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="62"/>
-      <c r="D11" s="50" t="s">
+      <c r="C11" s="47"/>
+      <c r="D11" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="51"/>
-      <c r="F11" s="52"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="29"/>
     </row>
     <row r="12" spans="2:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="8"/>
@@ -1982,77 +1980,77 @@
       <c r="F12" s="18"/>
     </row>
     <row r="13" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="42" t="s">
+      <c r="B13" s="74" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="38"/>
-      <c r="D13" s="38"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="39"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="50"/>
+      <c r="F13" s="51"/>
     </row>
     <row r="14" spans="2:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="40" t="s">
+      <c r="B14" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="33" t="s">
+      <c r="C14" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="35"/>
-      <c r="E14" s="33" t="s">
+      <c r="D14" s="40"/>
+      <c r="E14" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="34"/>
+      <c r="F14" s="39"/>
     </row>
     <row r="15" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="41"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="34"/>
+      <c r="B15" s="53"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="39"/>
     </row>
     <row r="16" spans="2:7" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="15">
         <v>1</v>
       </c>
-      <c r="C16" s="22"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="22" t="s">
+      <c r="C16" s="71"/>
+      <c r="D16" s="72"/>
+      <c r="E16" s="71" t="s">
         <v>37</v>
       </c>
-      <c r="F16" s="32"/>
+      <c r="F16" s="73"/>
     </row>
     <row r="17" spans="2:6" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="53">
+      <c r="B17" s="23">
         <v>2</v>
       </c>
-      <c r="C17" s="22" t="s">
+      <c r="C17" s="71" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="23"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="32"/>
+      <c r="D17" s="72"/>
+      <c r="E17" s="71"/>
+      <c r="F17" s="73"/>
     </row>
     <row r="18" spans="2:6" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="53">
+      <c r="B18" s="23">
         <v>3</v>
       </c>
-      <c r="C18" s="22"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="22" t="s">
+      <c r="C18" s="71"/>
+      <c r="D18" s="72"/>
+      <c r="E18" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="F18" s="32"/>
+      <c r="F18" s="73"/>
     </row>
     <row r="19" spans="2:6" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="16">
         <v>4</v>
       </c>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24" t="s">
+      <c r="C19" s="69"/>
+      <c r="D19" s="69"/>
+      <c r="E19" s="69" t="s">
         <v>40</v>
       </c>
-      <c r="F19" s="25"/>
+      <c r="F19" s="70"/>
     </row>
     <row r="20" spans="2:6" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="8"/>
@@ -2062,20 +2060,20 @@
       <c r="F20" s="18"/>
     </row>
     <row r="21" spans="2:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="37" t="s">
+      <c r="B21" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="38"/>
-      <c r="D21" s="39"/>
+      <c r="C21" s="50"/>
+      <c r="D21" s="51"/>
       <c r="E21" s="18"/>
       <c r="F21" s="18"/>
     </row>
     <row r="22" spans="2:6" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="71" t="s">
+      <c r="B22" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="C22" s="51"/>
-      <c r="D22" s="52"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="29"/>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
     </row>
@@ -2123,12 +2121,18 @@
     <row r="34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:F11"/>
     <mergeCell ref="B21:D21"/>
     <mergeCell ref="B22:D22"/>
     <mergeCell ref="B13:F13"/>
@@ -2137,18 +2141,12 @@
     <mergeCell ref="E14:F15"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="E16:F16"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>